<commit_message>
Sistemato e riorganizzato il DataPath
</commit_message>
<xml_diff>
--- a/DOCS/Tabella_FSM.xlsx
+++ b/DOCS/Tabella_FSM.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23706"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23713"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C613C235-194B-4B8C-8783-D5F3C9A900CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1D54218-32DA-4581-AE4B-C7418ECE49F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -646,8 +646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:Q58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2220,7 +2220,7 @@
         <v>15</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L43" s="2">
         <v>0</v>

</xml_diff>